<commit_message>
data: finalize revenue analysis dataset with cleaned formatting
</commit_message>
<xml_diff>
--- a/data/processed/revenue and profit margin.xlsx
+++ b/data/processed/revenue and profit margin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\tesla-optimus-business-analysis\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550C5409-462E-4D14-9A32-1537D0FC24EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3A4210-7EAC-4508-94F9-C9F036EE3ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -289,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -297,9 +297,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -309,9 +306,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -324,24 +318,9 @@
     <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -354,9 +333,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -372,12 +348,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -399,23 +369,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,324 +658,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="19.149999999999999">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2">
         <v>2024</v>
       </c>
-      <c r="C1" s="3"/>
+      <c r="C1" s="2">
+        <v>2023</v>
+      </c>
       <c r="D1" s="2">
-        <v>2023</v>
-      </c>
-      <c r="E1" s="2"/>
+        <v>2022</v>
+      </c>
+      <c r="E1" s="3">
+        <v>2021</v>
+      </c>
       <c r="F1" s="2">
-        <v>2022</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="4">
-        <v>2021</v>
-      </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="2">
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="19.149999999999999">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:6" ht="19.149999999999999">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="6"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" ht="19.149999999999999">
-      <c r="A3" s="10" t="s">
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="9">
         <v>72480</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="16"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="18">
+      <c r="F3" s="11">
         <v>26184</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="19.149999999999999">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20" t="s">
+      <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="20" t="s">
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="23"/>
-    </row>
-    <row r="5" spans="1:12" ht="19.149999999999999">
-      <c r="A5" s="10" t="s">
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24" t="s">
+      <c r="D5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="24" t="s">
+      <c r="E5" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="25">
+      <c r="F5" s="17">
         <v>1052</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="19.149999999999999">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27" t="s">
+      <c r="D6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27" t="s">
+      <c r="E6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="30">
+      <c r="F6" s="20">
         <v>27236</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="19.149999999999999">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="D7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="31">
+      <c r="F7" s="21">
         <v>1994</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="19.149999999999999">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="32" t="s">
+      <c r="C8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32" t="s">
+      <c r="D8" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="32"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="33">
+      <c r="E8" s="23">
         <v>3802</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="34">
+      <c r="F8" s="24">
         <v>2306</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="19.149999999999999">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36" t="s">
+      <c r="D9" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38">
+      <c r="E9" s="27">
         <v>53823</v>
       </c>
-      <c r="J9" s="36"/>
-      <c r="L9" s="38">
+      <c r="F9" s="27">
         <v>31536</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="19.149999999999999">
-      <c r="A10" s="19"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="9"/>
-    </row>
-    <row r="11" spans="1:12" ht="19.149999999999999">
-      <c r="A11" s="39" t="s">
+    <row r="10" spans="1:6" ht="19.149999999999999">
+      <c r="A10" s="12"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36" t="s">
+      <c r="D11" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="36"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="36" t="s">
+      <c r="E11" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="36"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="36">
+      <c r="F11" s="26">
         <v>862</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="23.25">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:6" ht="23.25">
+      <c r="A12" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="32">
+      <c r="C12" s="22">
         <v>-23</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32" t="s">
+      <c r="D12" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="32"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="32" t="s">
+      <c r="E12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="J12" s="32"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="32">
+      <c r="F12" s="22">
         <v>141</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="46.5">
-      <c r="A13" s="39" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="29">
         <v>7091</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="36" t="s">
+      <c r="C13" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="36" t="s">
+      <c r="D13" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="36" t="s">
+      <c r="E13" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="41"/>
-      <c r="L13" s="36">
+      <c r="F13" s="26">
         <v>721</v>
       </c>
     </row>

</xml_diff>